<commit_message>
Modified thermoPlotter to display thermocouple data from a control, 37.5mm quartz tube, and 52.2mm quartz tube. Results show quartz tube has no effect
</commit_message>
<xml_diff>
--- a/GravityPlunger Position vs Time Curve.xlsx
+++ b/GravityPlunger Position vs Time Curve.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Box\b - Time resolved crystallography\d - plunge cooler designs\d - plunge cooler v6 - Nathan design\gravity plunger IR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/82e9af8e6ee0abc9/Documents/Thorne Lab/Gravity-Plunger/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3069D1F5-5671-45A4-B43C-FE92FADDADFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{B7D5DD2E-D2A2-4B29-AEE6-30CFFB7CC8D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDA1AB33-20C6-4544-9E9C-19353C8EFB3A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{AB154802-62F5-4ED1-B1CD-C9AC497D3633}"/>
   </bookViews>
@@ -413,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2506260B-D9F9-43BD-8A02-3CB831456025}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -434,297 +434,361 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="B2">
-        <v>295</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="B3">
-        <v>272</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>568</v>
+        <v>572</v>
       </c>
       <c r="B4">
-        <v>258</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>566</v>
+        <v>571</v>
       </c>
       <c r="B5">
-        <v>235</v>
+        <v>286</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>564</v>
+        <v>570</v>
       </c>
       <c r="B6">
-        <v>223</v>
+        <v>272</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>562</v>
+        <v>569</v>
       </c>
       <c r="B7">
-        <v>213</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>560</v>
+        <v>568</v>
       </c>
       <c r="B8">
-        <v>205</v>
+        <v>258</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>558</v>
+        <v>567</v>
       </c>
       <c r="B9">
-        <v>200</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>556</v>
+        <v>566</v>
       </c>
       <c r="B10">
-        <v>195</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>554</v>
+        <v>565</v>
       </c>
       <c r="B11">
-        <v>190</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>552</v>
+        <v>564</v>
       </c>
       <c r="B12">
-        <v>186</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>550</v>
+        <v>563</v>
       </c>
       <c r="B13">
-        <v>183</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>548</v>
+        <v>562</v>
       </c>
       <c r="B14">
-        <v>180</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>546</v>
+        <v>561</v>
       </c>
       <c r="B15">
-        <v>176</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>544</v>
+        <v>560</v>
       </c>
       <c r="B16">
-        <v>172</v>
+        <v>205</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>542</v>
+        <v>558</v>
       </c>
       <c r="B17">
-        <v>169</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>540</v>
+        <v>556</v>
       </c>
       <c r="B18">
-        <v>166</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>530</v>
+        <v>554</v>
       </c>
       <c r="B19">
-        <v>153</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>520</v>
+        <v>552</v>
       </c>
       <c r="B20">
-        <v>141</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>510</v>
+        <v>550</v>
       </c>
       <c r="B21">
-        <v>130</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>500</v>
+        <v>548</v>
       </c>
       <c r="B22">
-        <v>120</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>490</v>
+        <v>546</v>
       </c>
       <c r="B23">
-        <v>111</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>480</v>
+        <v>544</v>
       </c>
       <c r="B24">
-        <v>103</v>
+        <v>172</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>470</v>
+        <v>542</v>
       </c>
       <c r="B25">
-        <v>95</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>460</v>
+        <v>540</v>
       </c>
       <c r="B26">
-        <v>88</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>450</v>
+        <v>530</v>
       </c>
       <c r="B27">
-        <v>80</v>
+        <v>153</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>440</v>
+        <v>520</v>
       </c>
       <c r="B28">
-        <v>73</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>430</v>
+        <v>510</v>
       </c>
       <c r="B29">
-        <v>66</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>420</v>
+        <v>500</v>
       </c>
       <c r="B30">
-        <v>60</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>410</v>
+        <v>490</v>
       </c>
       <c r="B31">
-        <v>53</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>400</v>
+        <v>480</v>
       </c>
       <c r="B32">
-        <v>48</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>390</v>
+        <v>470</v>
       </c>
       <c r="B33">
-        <v>42</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>380</v>
+        <v>460</v>
       </c>
       <c r="B34">
-        <v>36</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>370</v>
+        <v>450</v>
       </c>
       <c r="B35">
-        <v>31</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>360</v>
+        <v>440</v>
       </c>
       <c r="B36">
-        <v>25</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>350</v>
+        <v>430</v>
       </c>
       <c r="B37">
-        <v>20</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
+        <v>420</v>
+      </c>
+      <c r="B38">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>410</v>
+      </c>
+      <c r="B39">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>400</v>
+      </c>
+      <c r="B40">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>390</v>
+      </c>
+      <c r="B41">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>380</v>
+      </c>
+      <c r="B42">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>370</v>
+      </c>
+      <c r="B43">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>360</v>
+      </c>
+      <c r="B44">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>350</v>
+      </c>
+      <c r="B45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46">
         <v>340</v>
       </c>
-      <c r="B38">
+      <c r="B46">
         <v>15</v>
       </c>
     </row>

</xml_diff>